<commit_message>
progress for march 3
</commit_message>
<xml_diff>
--- a/YPI Data.xlsx
+++ b/YPI Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\magang-ypi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C90FD36-68D0-4E1C-9AE6-40520374B551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D16C84-9B53-455C-AB09-DC97707DCC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1727" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="183">
   <si>
     <t>USAID Projected 2050 value of losses due to sea level rise (in juta IDR)</t>
   </si>
@@ -674,6 +674,12 @@
   <si>
     <t>Hasil</t>
   </si>
+  <si>
+    <t>Luas Potensi</t>
+  </si>
+  <si>
+    <t>Luas Potensi Rusak</t>
+  </si>
 </sst>
 </file>
 
@@ -835,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -893,18 +899,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1187,1449 +1189,1539 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C254916-AD51-461C-A31D-B6AA1DD673EF}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="27"/>
+    <col min="1" max="1" width="20.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" style="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="E1" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="F1" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="I1" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="J1" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="L1" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="P1" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="O1" s="30"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="Q1" s="30"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="27" t="str">
+        <f>'Luas Terumbu Karang'!G39</f>
+        <v/>
+      </c>
+      <c r="E2" s="27" t="str">
+        <f>'Padang Lamun'!G39</f>
+        <v/>
+      </c>
+      <c r="F2" s="27" t="str">
+        <f>'Luas Mangove'!F39</f>
+        <v/>
+      </c>
+      <c r="G2" s="27" t="str">
+        <f>IF(COUNT(D2:F2)=0,"",SUM(D2:F2)/COUNT(D2:F2))</f>
+        <v/>
+      </c>
+      <c r="I2" s="27">
+        <f>'Korban Bencana Alam'!H42</f>
+        <v>2</v>
+      </c>
+      <c r="J2" s="27">
+        <f>IF(COUNT(I2)=0,"",SUM(I2)/COUNT(I2))</f>
+        <v>2</v>
+      </c>
+      <c r="L2" s="27">
+        <f>'Indeks Provinsi Membangun'!C39</f>
+        <v>3</v>
+      </c>
+      <c r="P2" s="27">
+        <f>SUM(G2,J2,L2)/COUNT(G2,J2,L2)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A3" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="27">
+        <f>'Luas Terumbu Karang'!G36</f>
+        <v>3</v>
+      </c>
+      <c r="E3" s="27">
+        <f>'Padang Lamun'!G36</f>
+        <v>3</v>
+      </c>
+      <c r="F3" s="27">
+        <f>'Luas Mangove'!F36</f>
+        <v>3</v>
+      </c>
+      <c r="G3" s="27">
+        <f>IF(COUNT(D3:F3)=0,"",SUM(D3:F3)/COUNT(D3:F3))</f>
+        <v>3</v>
+      </c>
+      <c r="I3" s="27">
+        <f>'Korban Bencana Alam'!H39</f>
+        <v>2</v>
+      </c>
+      <c r="J3" s="27">
+        <f>IF(COUNT(I3)=0,"",SUM(I3)/COUNT(I3))</f>
+        <v>2</v>
+      </c>
+      <c r="L3" s="27">
+        <f>'Indeks Provinsi Membangun'!C36</f>
+        <v>2</v>
+      </c>
+      <c r="P3" s="27">
+        <f>(G3+J3+L3)/COUNT(G3,J3,L3)</f>
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="27" t="str">
+        <f>'Luas Terumbu Karang'!G37</f>
+        <v/>
+      </c>
+      <c r="E4" s="27" t="str">
+        <f>'Padang Lamun'!G37</f>
+        <v/>
+      </c>
+      <c r="F4" s="27">
+        <f>'Luas Mangove'!F37</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="27">
+        <f>IF(COUNT(D4:F4)=0,"",SUM(D4:F4)/COUNT(D4:F4))</f>
+        <v>3</v>
+      </c>
+      <c r="I4" s="27">
+        <f>'Korban Bencana Alam'!H40</f>
+        <v>2</v>
+      </c>
+      <c r="J4" s="27">
+        <f>IF(COUNT(I4)=0,"",SUM(I4)/COUNT(I4))</f>
+        <v>2</v>
+      </c>
+      <c r="L4" s="27">
+        <f>'Indeks Provinsi Membangun'!C37</f>
+        <v>2</v>
+      </c>
+      <c r="P4" s="27">
+        <f>(G4+J4+L4)/COUNT(G4,J4,L4)</f>
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="27" t="str">
+        <f>'Luas Terumbu Karang'!G38</f>
+        <v/>
+      </c>
+      <c r="E5" s="27" t="str">
+        <f>'Padang Lamun'!G38</f>
+        <v/>
+      </c>
+      <c r="F5" s="27">
+        <f>'Luas Mangove'!F38</f>
+        <v>3</v>
+      </c>
+      <c r="G5" s="27">
+        <f>IF(COUNT(D5:F5)=0,"",SUM(D5:F5)/COUNT(D5:F5))</f>
+        <v>3</v>
+      </c>
+      <c r="I5" s="27">
+        <f>'Korban Bencana Alam'!H41</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="27">
+        <f>IF(COUNT(I5)=0,"",SUM(I5)/COUNT(I5))</f>
+        <v>1</v>
+      </c>
+      <c r="L5" s="27">
+        <f>'Indeks Provinsi Membangun'!C38</f>
+        <v>3</v>
+      </c>
+      <c r="P5" s="27">
+        <f>(G5+J5+L5)/COUNT(G5,J5,L5)</f>
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A6" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="27">
+        <f>'Luas Terumbu Karang'!G21</f>
+        <v>3</v>
+      </c>
+      <c r="E6" s="27">
+        <f>'Padang Lamun'!G21</f>
+        <v>3</v>
+      </c>
+      <c r="F6" s="27">
+        <f>'Luas Mangove'!F21</f>
+        <v>3</v>
+      </c>
+      <c r="G6" s="27">
+        <f>IF(COUNT(D6:F6)=0,"",SUM(D6:F6)/COUNT(D6:F6))</f>
+        <v>3</v>
+      </c>
+      <c r="I6" s="27">
+        <f>'Korban Bencana Alam'!H24</f>
+        <v>3</v>
+      </c>
+      <c r="J6" s="27">
+        <f>IF(COUNT(I6)=0,"",SUM(I6)/COUNT(I6))</f>
+        <v>3</v>
+      </c>
+      <c r="L6" s="27">
+        <f>'Indeks Provinsi Membangun'!C21</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="27">
+        <f>(G6+J6+L6)/COUNT(G6,J6,L6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A7" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="27">
+        <f>'Luas Terumbu Karang'!G3</f>
+        <v>3</v>
+      </c>
+      <c r="E7" s="27">
+        <f>'Padang Lamun'!G3</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="27">
+        <f>'Luas Mangove'!F3</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="27">
+        <f>IF(COUNT(D7:F7)=0,"",SUM(D7:F7)/COUNT(D7:F7))</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I7" s="27">
+        <f>'Korban Bencana Alam'!H6</f>
+        <v>3</v>
+      </c>
+      <c r="J7" s="27">
+        <f>IF(COUNT(I7)=0,"",SUM(I7)/COUNT(I7))</f>
+        <v>3</v>
+      </c>
+      <c r="L7" s="27">
+        <f>'Indeks Provinsi Membangun'!C3</f>
+        <v>1</v>
+      </c>
+      <c r="P7" s="27">
+        <f>(G7+J7+L7)/COUNT(G7,J7,L7)</f>
+        <v>1.8888888888888891</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A8" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="27">
+        <f>'Luas Terumbu Karang'!G28</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="27">
+        <f>'Padang Lamun'!G28</f>
+        <v>3</v>
+      </c>
+      <c r="F8" s="27">
+        <f>'Luas Mangove'!F28</f>
+        <v>2</v>
+      </c>
+      <c r="G8" s="27">
+        <f>IF(COUNT(D8:F8)=0,"",SUM(D8:F8)/COUNT(D8:F8))</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="I8" s="27">
+        <f>'Korban Bencana Alam'!H31</f>
+        <v>3</v>
+      </c>
+      <c r="J8" s="27">
+        <f>IF(COUNT(I8)=0,"",SUM(I8)/COUNT(I8))</f>
+        <v>3</v>
+      </c>
+      <c r="L8" s="27">
+        <f>'Indeks Provinsi Membangun'!C28</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="27">
+        <f>(G8+J8+L8)/COUNT(G8,J8,L8)</f>
+        <v>1.8888888888888886</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A9" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="27">
+        <f>'Luas Terumbu Karang'!G20</f>
+        <v>3</v>
+      </c>
+      <c r="E9" s="27">
+        <f>'Padang Lamun'!G20</f>
+        <v>3</v>
+      </c>
+      <c r="F9" s="27">
+        <f>'Luas Mangove'!F20</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="27">
+        <f>IF(COUNT(D9:F9)=0,"",SUM(D9:F9)/COUNT(D9:F9))</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="I9" s="27">
+        <f>'Korban Bencana Alam'!H23</f>
+        <v>2</v>
+      </c>
+      <c r="J9" s="27">
+        <f>IF(COUNT(I9)=0,"",SUM(I9)/COUNT(I9))</f>
+        <v>2</v>
+      </c>
+      <c r="L9" s="27">
+        <f>'Indeks Provinsi Membangun'!C20</f>
+        <v>1</v>
+      </c>
+      <c r="P9" s="27">
+        <f>(G9+J9+L9)/COUNT(G9,J9,L9)</f>
+        <v>1.7777777777777779</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="27" t="str">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="27" t="str">
         <f>'Luas Terumbu Karang'!G2</f>
         <v/>
       </c>
-      <c r="C2" s="27" t="str">
+      <c r="E10" s="27" t="str">
         <f>'Padang Lamun'!G2</f>
         <v/>
       </c>
-      <c r="D2" s="27">
+      <c r="F10" s="27">
         <f>'Luas Mangove'!F2</f>
         <v>1</v>
       </c>
-      <c r="E2" s="27">
-        <f>IF(COUNT(B2:D2)=0,"",SUM(B2:D2)/COUNT(B2:D2))</f>
-        <v>1</v>
-      </c>
-      <c r="G2" s="27">
+      <c r="G10" s="27">
+        <f>IF(COUNT(D10:F10)=0,"",SUM(D10:F10)/COUNT(D10:F10))</f>
+        <v>1</v>
+      </c>
+      <c r="I10" s="27">
         <f>'Korban Bencana Alam'!H5</f>
         <v>3</v>
       </c>
-      <c r="H2" s="27">
-        <f>IF(COUNT(G2)=0,"",SUM(G2)/COUNT(G2))</f>
+      <c r="J10" s="27">
+        <f>IF(COUNT(I10)=0,"",SUM(I10)/COUNT(I10))</f>
         <v>3</v>
       </c>
-      <c r="J2" s="27">
+      <c r="L10" s="27">
         <f>'Indeks Provinsi Membangun'!C2</f>
         <v>1</v>
       </c>
-      <c r="N2" s="27">
-        <f t="shared" ref="N2:N38" si="0">(E2+H2+J2)/COUNT(E2,H2,J2)</f>
+      <c r="P10" s="27">
+        <f>(G10+J10+L10)/COUNT(G10,J10,L10)</f>
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A3" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="27">
-        <f>'Luas Terumbu Karang'!G3</f>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A11" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="27">
+        <f>'Luas Terumbu Karang'!G16</f>
+        <v>2</v>
+      </c>
+      <c r="E11" s="27">
+        <f>'Padang Lamun'!G16</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="27">
+        <f>'Luas Mangove'!F16</f>
+        <v>2</v>
+      </c>
+      <c r="G11" s="27">
+        <f>IF(COUNT(D11:F11)=0,"",SUM(D11:F11)/COUNT(D11:F11))</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I11" s="27">
+        <f>'Korban Bencana Alam'!H19</f>
         <v>3</v>
       </c>
-      <c r="C3" s="27">
-        <f>'Padang Lamun'!G3</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="27">
-        <f>'Luas Mangove'!F3</f>
+      <c r="J11" s="27">
+        <f>IF(COUNT(I11)=0,"",SUM(I11)/COUNT(I11))</f>
+        <v>3</v>
+      </c>
+      <c r="L11" s="27">
+        <f>'Indeks Provinsi Membangun'!C16</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="27">
+        <f>(G11+J11+L11)/COUNT(G11,J11,L11)</f>
+        <v>1.5555555555555556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A12" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="27">
+        <f>'Luas Terumbu Karang'!G24</f>
+        <v>3</v>
+      </c>
+      <c r="E12" s="27">
+        <f>'Padang Lamun'!G24</f>
         <v>2</v>
       </c>
-      <c r="E3" s="27">
-        <f t="shared" ref="E3:E39" si="1">IF(COUNT(B3:D3)=0,"",SUM(B3:D3)/COUNT(B3:D3))</f>
+      <c r="F12" s="27">
+        <f>'Luas Mangove'!F24</f>
+        <v>3</v>
+      </c>
+      <c r="G12" s="27">
+        <f>IF(COUNT(D12:F12)=0,"",SUM(D12:F12)/COUNT(D12:F12))</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="I12" s="27">
+        <f>'Korban Bencana Alam'!H27</f>
+        <v>2</v>
+      </c>
+      <c r="J12" s="27">
+        <f>IF(COUNT(I12)=0,"",SUM(I12)/COUNT(I12))</f>
+        <v>2</v>
+      </c>
+      <c r="L12" s="27">
+        <f>'Indeks Provinsi Membangun'!C24</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="27">
+        <f>(G12+J12+L12)/COUNT(G12,J12,L12)</f>
+        <v>1.5555555555555554</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A13" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="27">
+        <f>'Luas Terumbu Karang'!G14</f>
+        <v>2</v>
+      </c>
+      <c r="E13" s="27">
+        <f>'Padang Lamun'!G14</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="27">
+        <f>'Luas Mangove'!F14</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="27">
+        <f>IF(COUNT(D13:F13)=0,"",SUM(D13:F13)/COUNT(D13:F13))</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I13" s="27">
+        <f>'Korban Bencana Alam'!H17</f>
+        <v>3</v>
+      </c>
+      <c r="J13" s="27">
+        <f>IF(COUNT(I13)=0,"",SUM(I13)/COUNT(I13))</f>
+        <v>3</v>
+      </c>
+      <c r="L13" s="27">
+        <f>'Indeks Provinsi Membangun'!C14</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="27">
+        <f>(G13+J13+L13)/COUNT(G13,J13,L13)</f>
+        <v>1.4444444444444444</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A14" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="27">
+        <f>'Luas Terumbu Karang'!G23</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="27">
+        <f>'Padang Lamun'!G23</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="27">
+        <f>'Luas Mangove'!F23</f>
+        <v>2</v>
+      </c>
+      <c r="G14" s="27">
+        <f>IF(COUNT(D14:F14)=0,"",SUM(D14:F14)/COUNT(D14:F14))</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I14" s="27">
+        <f>'Korban Bencana Alam'!H26</f>
+        <v>3</v>
+      </c>
+      <c r="J14" s="27">
+        <f>IF(COUNT(I14)=0,"",SUM(I14)/COUNT(I14))</f>
+        <v>3</v>
+      </c>
+      <c r="L14" s="27">
+        <f>'Indeks Provinsi Membangun'!C23</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="27">
+        <f>(G14+J14+L14)/COUNT(G14,J14,L14)</f>
+        <v>1.4444444444444444</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A15" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="27">
+        <f>'Luas Terumbu Karang'!G5</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="27">
+        <f>'Padang Lamun'!G5</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="27">
+        <f>'Luas Mangove'!F5</f>
+        <v>3</v>
+      </c>
+      <c r="G15" s="27">
+        <f>IF(COUNT(D15:F15)=0,"",SUM(D15:F15)/COUNT(D15:F15))</f>
+        <v>1</v>
+      </c>
+      <c r="I15" s="27">
+        <f>'Korban Bencana Alam'!H8</f>
+        <v>3</v>
+      </c>
+      <c r="J15" s="27">
+        <f>IF(COUNT(I15)=0,"",SUM(I15)/COUNT(I15))</f>
+        <v>3</v>
+      </c>
+      <c r="L15" s="27">
+        <f>'Indeks Provinsi Membangun'!C5</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="27">
+        <f>(G15+J15+L15)/COUNT(G15,J15,L15)</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="27" t="str">
+        <f>'Luas Terumbu Karang'!G13</f>
+        <v/>
+      </c>
+      <c r="E16" s="27" t="str">
+        <f>'Padang Lamun'!G13</f>
+        <v/>
+      </c>
+      <c r="F16" s="27">
+        <f>'Luas Mangove'!F13</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="27">
+        <f>IF(COUNT(D16:F16)=0,"",SUM(D16:F16)/COUNT(D16:F16))</f>
+        <v>1</v>
+      </c>
+      <c r="I16" s="27">
+        <f>'Korban Bencana Alam'!H16</f>
+        <v>3</v>
+      </c>
+      <c r="J16" s="27">
+        <f>IF(COUNT(I16)=0,"",SUM(I16)/COUNT(I16))</f>
+        <v>3</v>
+      </c>
+      <c r="L16" s="27">
+        <f>'Indeks Provinsi Membangun'!C13</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="27">
+        <f>(G16+J16+L16)/COUNT(G16,J16,L16)</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A17" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="27">
+        <f>'Luas Terumbu Karang'!G25</f>
+        <v>3</v>
+      </c>
+      <c r="E17" s="27">
+        <f>'Padang Lamun'!G25</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="27">
+        <f>'Luas Mangove'!F25</f>
+        <v>3</v>
+      </c>
+      <c r="G17" s="27">
+        <f>IF(COUNT(D17:F17)=0,"",SUM(D17:F17)/COUNT(D17:F17))</f>
+        <v>2</v>
+      </c>
+      <c r="I17" s="27">
+        <f>'Korban Bencana Alam'!H28</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="27">
+        <f>IF(COUNT(I17)=0,"",SUM(I17)/COUNT(I17))</f>
+        <v>1</v>
+      </c>
+      <c r="L17" s="27">
+        <f>'Indeks Provinsi Membangun'!C25</f>
+        <v>1</v>
+      </c>
+      <c r="P17" s="27">
+        <f>(G17+J17+L17)/COUNT(G17,J17,L17)</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A18" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="27">
+        <f>'Luas Terumbu Karang'!G32</f>
+        <v>3</v>
+      </c>
+      <c r="E18" s="27">
+        <f>'Padang Lamun'!G32</f>
+        <v>3</v>
+      </c>
+      <c r="F18" s="27">
+        <f>'Luas Mangove'!F32</f>
+        <v>3</v>
+      </c>
+      <c r="G18" s="27">
+        <f>IF(COUNT(D18:F18)=0,"",SUM(D18:F18)/COUNT(D18:F18))</f>
+        <v>3</v>
+      </c>
+      <c r="I18" s="27">
+        <f>'Korban Bencana Alam'!H35</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="27">
+        <f>IF(COUNT(I18)=0,"",SUM(I18)/COUNT(I18))</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="27">
+        <f>'Indeks Provinsi Membangun'!C32</f>
+        <v>1</v>
+      </c>
+      <c r="P18" s="27">
+        <f>(G18+J18+L18)/COUNT(G18,J18,L18)</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="27" t="str">
+        <f>'Luas Terumbu Karang'!G35</f>
+        <v/>
+      </c>
+      <c r="E19" s="27" t="str">
+        <f>'Padang Lamun'!G35</f>
+        <v/>
+      </c>
+      <c r="F19" s="27">
+        <f>'Luas Mangove'!F35</f>
+        <v>2</v>
+      </c>
+      <c r="G19" s="27">
+        <f>IF(COUNT(D19:F19)=0,"",SUM(D19:F19)/COUNT(D19:F19))</f>
+        <v>2</v>
+      </c>
+      <c r="I19" s="27">
+        <f>'Korban Bencana Alam'!H38</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="27">
+        <f>IF(COUNT(I19)=0,"",SUM(I19)/COUNT(I19))</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="27">
+        <f>'Indeks Provinsi Membangun'!C35</f>
+        <v>2</v>
+      </c>
+      <c r="P19" s="27">
+        <f>(G19+J19+L19)/COUNT(G19,J19,L19)</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A20" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="27">
+        <f>'Luas Terumbu Karang'!G19</f>
+        <v>2</v>
+      </c>
+      <c r="E20" s="27">
+        <f>'Padang Lamun'!G19</f>
+        <v>2</v>
+      </c>
+      <c r="F20" s="27">
+        <f>'Luas Mangove'!F19</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="27">
+        <f>IF(COUNT(D20:F20)=0,"",SUM(D20:F20)/COUNT(D20:F20))</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="G3" s="27">
-        <f>'Korban Bencana Alam'!H6</f>
+      <c r="I20" s="27">
+        <f>'Korban Bencana Alam'!H22</f>
+        <v>2</v>
+      </c>
+      <c r="J20" s="27">
+        <f>IF(COUNT(I20)=0,"",SUM(I20)/COUNT(I20))</f>
+        <v>2</v>
+      </c>
+      <c r="L20" s="27">
+        <f>'Indeks Provinsi Membangun'!C19</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="27">
+        <f>(G20+J20+L20)/COUNT(G20,J20,L20)</f>
+        <v>1.2222222222222223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A21" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="27">
+        <f>'Luas Terumbu Karang'!G34</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="27">
+        <f>'Padang Lamun'!G34</f>
+        <v>2</v>
+      </c>
+      <c r="F21" s="27">
+        <f>'Luas Mangove'!F34</f>
         <v>3</v>
       </c>
-      <c r="H3" s="27">
-        <f t="shared" ref="H3:H39" si="2">IF(COUNT(G3)=0,"",SUM(G3)/COUNT(G3))</f>
+      <c r="G21" s="27">
+        <f>IF(COUNT(D21:F21)=0,"",SUM(D21:F21)/COUNT(D21:F21))</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I21" s="27">
+        <f>'Korban Bencana Alam'!H37</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="27">
+        <f>IF(COUNT(I21)=0,"",SUM(I21)/COUNT(I21))</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="27">
+        <f>'Indeks Provinsi Membangun'!C34</f>
+        <v>2</v>
+      </c>
+      <c r="P21" s="27">
+        <f>(G21+J21+L21)/COUNT(G21,J21,L21)</f>
+        <v>1.2222222222222223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A22" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="27">
+        <f>'Luas Terumbu Karang'!G22</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="27">
+        <f>'Padang Lamun'!G22</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="27">
+        <f>'Luas Mangove'!F22</f>
+        <v>2</v>
+      </c>
+      <c r="G22" s="27">
+        <f>IF(COUNT(D22:F22)=0,"",SUM(D22:F22)/COUNT(D22:F22))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I22" s="27">
+        <f>'Korban Bencana Alam'!H25</f>
         <v>3</v>
       </c>
-      <c r="J3" s="27">
-        <f>'Indeks Provinsi Membangun'!C3</f>
-        <v>1</v>
-      </c>
-      <c r="N3" s="27">
-        <f t="shared" si="0"/>
-        <v>1.8888888888888891</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A4" s="33" t="s">
+      <c r="J22" s="27">
+        <f>IF(COUNT(I22)=0,"",SUM(I22)/COUNT(I22))</f>
+        <v>3</v>
+      </c>
+      <c r="L22" s="27">
+        <f>'Indeks Provinsi Membangun'!C22</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="27">
+        <f>(G22+J22+L22)/COUNT(G22,J22,L22)</f>
+        <v>1.2222222222222221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="27">
+        <f>'Luas Terumbu Karang'!G7</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="27" t="str">
+        <f>'Padang Lamun'!G7</f>
+        <v/>
+      </c>
+      <c r="F23" s="27">
+        <f>'Luas Mangove'!F7</f>
+        <v>3</v>
+      </c>
+      <c r="G23" s="27">
+        <f>IF(COUNT(D23:F23)=0,"",SUM(D23:F23)/COUNT(D23:F23))</f>
+        <v>1.5</v>
+      </c>
+      <c r="I23" s="27">
+        <f>'Korban Bencana Alam'!H10</f>
+        <v>1</v>
+      </c>
+      <c r="J23" s="27">
+        <f>IF(COUNT(I23)=0,"",SUM(I23)/COUNT(I23))</f>
+        <v>1</v>
+      </c>
+      <c r="L23" s="27">
+        <f>'Indeks Provinsi Membangun'!C7</f>
+        <v>1</v>
+      </c>
+      <c r="P23" s="27">
+        <f>(G23+J23+L23)/COUNT(G23,J23,L23)</f>
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A24" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="27">
         <f>'Luas Terumbu Karang'!G4</f>
         <v>2</v>
       </c>
-      <c r="C4" s="27">
+      <c r="E24" s="27">
         <f>'Padang Lamun'!G4</f>
         <v>1</v>
       </c>
-      <c r="D4" s="27">
+      <c r="F24" s="27">
         <f>'Luas Mangove'!F4</f>
         <v>1</v>
       </c>
-      <c r="E4" s="27">
-        <f t="shared" si="1"/>
+      <c r="G24" s="27">
+        <f>IF(COUNT(D24:F24)=0,"",SUM(D24:F24)/COUNT(D24:F24))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="G4" s="27">
+      <c r="I24" s="27">
         <f>'Korban Bencana Alam'!H7</f>
         <v>2</v>
       </c>
-      <c r="H4" s="27">
-        <f t="shared" si="2"/>
+      <c r="J24" s="27">
+        <f>IF(COUNT(I24)=0,"",SUM(I24)/COUNT(I24))</f>
         <v>2</v>
       </c>
-      <c r="J4" s="27">
+      <c r="L24" s="27">
         <f>'Indeks Provinsi Membangun'!C4</f>
         <v>0</v>
       </c>
-      <c r="N4" s="27">
-        <f t="shared" si="0"/>
+      <c r="P24" s="27">
+        <f>(G24+J24+L24)/COUNT(G24,J24,L24)</f>
         <v>1.1111111111111109</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A5" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="27">
-        <f>'Luas Terumbu Karang'!G5</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="27">
-        <f>'Padang Lamun'!G5</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="27">
-        <f>'Luas Mangove'!F5</f>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A25" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="27">
+        <f>'Luas Terumbu Karang'!G29</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="27">
+        <f>'Padang Lamun'!G29</f>
+        <v>2</v>
+      </c>
+      <c r="F25" s="27">
+        <f>'Luas Mangove'!F29</f>
+        <v>2</v>
+      </c>
+      <c r="G25" s="27">
+        <f>IF(COUNT(D25:F25)=0,"",SUM(D25:F25)/COUNT(D25:F25))</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I25" s="27">
+        <f>'Korban Bencana Alam'!H32</f>
+        <v>1</v>
+      </c>
+      <c r="J25" s="27">
+        <f>IF(COUNT(I25)=0,"",SUM(I25)/COUNT(I25))</f>
+        <v>1</v>
+      </c>
+      <c r="L25" s="27">
+        <f>'Indeks Provinsi Membangun'!C29</f>
+        <v>1</v>
+      </c>
+      <c r="P25" s="27">
+        <f>(G25+J25+L25)/COUNT(G25,J25,L25)</f>
+        <v>1.1111111111111109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A26" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="27">
+        <f>'Luas Terumbu Karang'!G17</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="27">
+        <f>'Padang Lamun'!G17</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="27">
+        <f>'Luas Mangove'!F17</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="27">
+        <f>IF(COUNT(D26:F26)=0,"",SUM(D26:F26)/COUNT(D26:F26))</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="27">
+        <f>'Korban Bencana Alam'!H20</f>
+        <v>2</v>
+      </c>
+      <c r="J26" s="27">
+        <f>IF(COUNT(I26)=0,"",SUM(I26)/COUNT(I26))</f>
+        <v>2</v>
+      </c>
+      <c r="L26" s="27">
+        <f>'Indeks Provinsi Membangun'!C17</f>
+        <v>1</v>
+      </c>
+      <c r="P26" s="27">
+        <f>(G26+J26+L26)/COUNT(G26,J26,L26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="27" t="str">
+        <f>'Luas Terumbu Karang'!G27</f>
+        <v/>
+      </c>
+      <c r="E27" s="27" t="str">
+        <f>'Padang Lamun'!G27</f>
+        <v/>
+      </c>
+      <c r="F27" s="27">
+        <f>'Luas Mangove'!F27</f>
+        <v>1</v>
+      </c>
+      <c r="G27" s="27">
+        <f>IF(COUNT(D27:F27)=0,"",SUM(D27:F27)/COUNT(D27:F27))</f>
+        <v>1</v>
+      </c>
+      <c r="I27" s="27">
+        <f>'Korban Bencana Alam'!H30</f>
+        <v>2</v>
+      </c>
+      <c r="J27" s="27">
+        <f>IF(COUNT(I27)=0,"",SUM(I27)/COUNT(I27))</f>
+        <v>2</v>
+      </c>
+      <c r="L27" s="27">
+        <f>'Indeks Provinsi Membangun'!C27</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="27">
+        <f>(G27+J27+L27)/COUNT(G27,J27,L27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A28" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="27">
+        <f>'Luas Terumbu Karang'!G33</f>
+        <v>2</v>
+      </c>
+      <c r="E28" s="27">
+        <f>'Padang Lamun'!G33</f>
         <v>3</v>
       </c>
-      <c r="E5" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G5" s="27">
-        <f>'Korban Bencana Alam'!H8</f>
+      <c r="F28" s="27">
+        <f>'Luas Mangove'!F33</f>
+        <v>1</v>
+      </c>
+      <c r="G28" s="27">
+        <f>IF(COUNT(D28:F28)=0,"",SUM(D28:F28)/COUNT(D28:F28))</f>
+        <v>2</v>
+      </c>
+      <c r="I28" s="27">
+        <f>'Korban Bencana Alam'!H36</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="27">
+        <f>IF(COUNT(I28)=0,"",SUM(I28)/COUNT(I28))</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="27">
+        <f>'Indeks Provinsi Membangun'!C33</f>
+        <v>1</v>
+      </c>
+      <c r="P28" s="27">
+        <f>(G28+J28+L28)/COUNT(G28,J28,L28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A29" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="27">
+        <f>'Luas Terumbu Karang'!G30</f>
+        <v>2</v>
+      </c>
+      <c r="E29" s="27">
+        <f>'Padang Lamun'!G30</f>
+        <v>2</v>
+      </c>
+      <c r="F29" s="27">
+        <f>'Luas Mangove'!F30</f>
+        <v>1</v>
+      </c>
+      <c r="G29" s="27">
+        <f>IF(COUNT(D29:F29)=0,"",SUM(D29:F29)/COUNT(D29:F29))</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I29" s="27">
+        <f>'Korban Bencana Alam'!H33</f>
+        <v>1</v>
+      </c>
+      <c r="J29" s="27">
+        <f>IF(COUNT(I29)=0,"",SUM(I29)/COUNT(I29))</f>
+        <v>1</v>
+      </c>
+      <c r="L29" s="27">
+        <f>'Indeks Provinsi Membangun'!C30</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="27">
+        <f>(G29+J29+L29)/COUNT(G29,J29,L29)</f>
+        <v>0.88888888888888895</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="27">
+        <f>'Luas Terumbu Karang'!G12</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="27">
+        <f>'Padang Lamun'!G12</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="27">
+        <f>'Luas Mangove'!F12</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="27">
+        <f>IF(COUNT(D30:F30)=0,"",SUM(D30:F30)/COUNT(D30:F30))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I30" s="27">
+        <f>'Korban Bencana Alam'!H15</f>
+        <v>1</v>
+      </c>
+      <c r="J30" s="27">
+        <f>IF(COUNT(I30)=0,"",SUM(I30)/COUNT(I30))</f>
+        <v>1</v>
+      </c>
+      <c r="P30" s="27">
+        <f>(G30+J30+L30)/COUNT(G30,J30,L30)</f>
+        <v>0.83333333333333326</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A31" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="27">
+        <f>'Luas Terumbu Karang'!G26</f>
+        <v>1</v>
+      </c>
+      <c r="E31" s="27">
+        <f>'Padang Lamun'!G26</f>
         <v>3</v>
       </c>
-      <c r="H5" s="27">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J5" s="27">
-        <f>'Indeks Provinsi Membangun'!C5</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="27">
-        <f t="shared" si="0"/>
+      <c r="F31" s="27">
+        <f>'Luas Mangove'!F26</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="27">
+        <f>IF(COUNT(D31:F31)=0,"",SUM(D31:F31)/COUNT(D31:F31))</f>
         <v>1.3333333333333333</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
+      <c r="I31" s="27">
+        <f>'Korban Bencana Alam'!H29</f>
+        <v>1</v>
+      </c>
+      <c r="J31" s="27">
+        <f>IF(COUNT(I31)=0,"",SUM(I31)/COUNT(I31))</f>
+        <v>1</v>
+      </c>
+      <c r="L31" s="27">
+        <f>'Indeks Provinsi Membangun'!C26</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="27">
+        <f>(G31+J31+L31)/COUNT(G31,J31,L31)</f>
+        <v>0.77777777777777768</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A32" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="27">
+        <f>'Luas Terumbu Karang'!G8</f>
+        <v>1</v>
+      </c>
+      <c r="E32" s="27">
+        <f>'Padang Lamun'!G8</f>
+        <v>2</v>
+      </c>
+      <c r="F32" s="27">
+        <f>'Luas Mangove'!F8</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="27">
+        <f>IF(COUNT(D32:F32)=0,"",SUM(D32:F32)/COUNT(D32:F32))</f>
+        <v>1</v>
+      </c>
+      <c r="I32" s="27">
+        <f>'Korban Bencana Alam'!H11</f>
+        <v>1</v>
+      </c>
+      <c r="J32" s="27">
+        <f>IF(COUNT(I32)=0,"",SUM(I32)/COUNT(I32))</f>
+        <v>1</v>
+      </c>
+      <c r="L32" s="27">
+        <f>'Indeks Provinsi Membangun'!C8</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="27">
+        <f>(G32+J32+L32)/COUNT(G32,J32,L32)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A33" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="27">
+        <f>'Luas Terumbu Karang'!G10</f>
+        <v>2</v>
+      </c>
+      <c r="E33" s="27">
+        <f>'Padang Lamun'!G10</f>
+        <v>2</v>
+      </c>
+      <c r="F33" s="27">
+        <f>'Luas Mangove'!F10</f>
+        <v>2</v>
+      </c>
+      <c r="G33" s="27">
+        <f>IF(COUNT(D33:F33)=0,"",SUM(D33:F33)/COUNT(D33:F33))</f>
+        <v>2</v>
+      </c>
+      <c r="I33" s="27">
+        <f>'Korban Bencana Alam'!H13</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="27">
+        <f>IF(COUNT(I33)=0,"",SUM(I33)/COUNT(I33))</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="27">
+        <f>'Indeks Provinsi Membangun'!C10</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="27">
+        <f>(G33+J33+L33)/COUNT(G33,J33,L33)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A34" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="27">
+        <f>'Luas Terumbu Karang'!G31</f>
+        <v>1</v>
+      </c>
+      <c r="E34" s="27">
+        <f>'Padang Lamun'!G31</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="27">
+        <f>'Luas Mangove'!F31</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="27">
+        <f>IF(COUNT(D34:F34)=0,"",SUM(D34:F34)/COUNT(D34:F34))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I34" s="27">
+        <f>'Korban Bencana Alam'!H34</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="27">
+        <f>IF(COUNT(I34)=0,"",SUM(I34)/COUNT(I34))</f>
+        <v>0</v>
+      </c>
+      <c r="L34" s="27">
+        <f>'Indeks Provinsi Membangun'!C31</f>
+        <v>1</v>
+      </c>
+      <c r="P34" s="27">
+        <f>(G34+J34+L34)/COUNT(G34,J34,L34)</f>
+        <v>0.55555555555555547</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="27" t="str">
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="27" t="str">
         <f>'Luas Terumbu Karang'!G6</f>
         <v/>
       </c>
-      <c r="C6" s="27" t="str">
+      <c r="E35" s="27" t="str">
         <f>'Padang Lamun'!G6</f>
         <v/>
       </c>
-      <c r="D6" s="27">
+      <c r="F35" s="27">
         <f>'Luas Mangove'!F6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="27">
+      <c r="G35" s="27">
+        <f>IF(COUNT(D35:F35)=0,"",SUM(D35:F35)/COUNT(D35:F35))</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="27">
         <f>'Korban Bencana Alam'!H9</f>
         <v>1</v>
       </c>
-      <c r="H6" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J6" s="27">
+      <c r="J35" s="27">
+        <f>IF(COUNT(I35)=0,"",SUM(I35)/COUNT(I35))</f>
+        <v>1</v>
+      </c>
+      <c r="L35" s="27">
         <f>'Indeks Provinsi Membangun'!C6</f>
         <v>0</v>
       </c>
-      <c r="N6" s="27">
-        <f t="shared" si="0"/>
+      <c r="P35" s="27">
+        <f>(G35+J35+L35)/COUNT(G35,J35,L35)</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="27">
-        <f>'Luas Terumbu Karang'!G7</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="27" t="str">
-        <f>'Padang Lamun'!G7</f>
-        <v/>
-      </c>
-      <c r="D7" s="27">
-        <f>'Luas Mangove'!F7</f>
-        <v>3</v>
-      </c>
-      <c r="E7" s="27">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="G7" s="27">
-        <f>'Korban Bencana Alam'!H10</f>
-        <v>1</v>
-      </c>
-      <c r="H7" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J7" s="27">
-        <f>'Indeks Provinsi Membangun'!C7</f>
-        <v>1</v>
-      </c>
-      <c r="N7" s="27">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A8" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="27">
-        <f>'Luas Terumbu Karang'!G8</f>
-        <v>1</v>
-      </c>
-      <c r="C8" s="27">
-        <f>'Padang Lamun'!G8</f>
-        <v>2</v>
-      </c>
-      <c r="D8" s="27">
-        <f>'Luas Mangove'!F8</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G8" s="27">
-        <f>'Korban Bencana Alam'!H11</f>
-        <v>1</v>
-      </c>
-      <c r="H8" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J8" s="27">
-        <f>'Indeks Provinsi Membangun'!C8</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="27">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A9" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="27">
-        <f>'Luas Terumbu Karang'!G9</f>
-        <v>1</v>
-      </c>
-      <c r="C9" s="27">
-        <f>'Padang Lamun'!G9</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="27">
-        <f>'Luas Mangove'!F9</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="27">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G9" s="27">
-        <f>'Korban Bencana Alam'!H12</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="27">
-        <f>'Indeks Provinsi Membangun'!C9</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="27">
-        <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A10" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="27">
-        <f>'Luas Terumbu Karang'!G10</f>
-        <v>2</v>
-      </c>
-      <c r="C10" s="27">
-        <f>'Padang Lamun'!G10</f>
-        <v>2</v>
-      </c>
-      <c r="D10" s="27">
-        <f>'Luas Mangove'!F10</f>
-        <v>2</v>
-      </c>
-      <c r="E10" s="27">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G10" s="27">
-        <f>'Korban Bencana Alam'!H13</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="27">
-        <f>'Indeks Provinsi Membangun'!C10</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="27">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A11" s="33" t="s">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A36" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="27">
         <f>'Luas Terumbu Karang'!G11</f>
         <v>0</v>
       </c>
-      <c r="C11" s="27">
+      <c r="E36" s="27">
         <f>'Padang Lamun'!G11</f>
         <v>0</v>
       </c>
-      <c r="D11" s="27">
+      <c r="F36" s="27">
         <f>'Luas Mangove'!F11</f>
         <v>2</v>
       </c>
-      <c r="E11" s="27">
-        <f t="shared" si="1"/>
+      <c r="G36" s="27">
+        <f>IF(COUNT(D36:F36)=0,"",SUM(D36:F36)/COUNT(D36:F36))</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G11" s="27">
+      <c r="I36" s="27">
         <f>'Korban Bencana Alam'!H14</f>
         <v>0</v>
       </c>
-      <c r="H11" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="27">
+      <c r="J36" s="27">
+        <f>IF(COUNT(I36)=0,"",SUM(I36)/COUNT(I36))</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="27">
         <f>'Indeks Provinsi Membangun'!C11</f>
         <v>0</v>
       </c>
-      <c r="N11" s="27">
-        <f t="shared" si="0"/>
+      <c r="P36" s="27">
+        <f>(G36+J36+L36)/COUNT(G36,J36,L36)</f>
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="27">
-        <f>'Luas Terumbu Karang'!G12</f>
-        <v>1</v>
-      </c>
-      <c r="C12" s="27">
-        <f>'Padang Lamun'!G12</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="27">
-        <f>'Luas Mangove'!F12</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="27">
-        <f t="shared" si="1"/>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A37" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="27">
+        <f>'Luas Terumbu Karang'!G18</f>
+        <v>1</v>
+      </c>
+      <c r="E37" s="27">
+        <f>'Padang Lamun'!G18</f>
+        <v>1</v>
+      </c>
+      <c r="F37" s="27">
+        <f>'Luas Mangove'!F18</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="27">
+        <f>IF(COUNT(D37:F37)=0,"",SUM(D37:F37)/COUNT(D37:F37))</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G12" s="27">
-        <f>'Korban Bencana Alam'!H15</f>
-        <v>1</v>
-      </c>
-      <c r="H12" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="N12" s="27">
-        <f t="shared" si="0"/>
-        <v>0.83333333333333326</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="27" t="str">
-        <f>'Luas Terumbu Karang'!G13</f>
-        <v/>
-      </c>
-      <c r="C13" s="27" t="str">
-        <f>'Padang Lamun'!G13</f>
-        <v/>
-      </c>
-      <c r="D13" s="27">
-        <f>'Luas Mangove'!F13</f>
-        <v>1</v>
-      </c>
-      <c r="E13" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G13" s="27">
-        <f>'Korban Bencana Alam'!H16</f>
-        <v>3</v>
-      </c>
-      <c r="H13" s="27">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J13" s="27">
-        <f>'Indeks Provinsi Membangun'!C13</f>
-        <v>0</v>
-      </c>
-      <c r="N13" s="27">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A14" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="27">
-        <f>'Luas Terumbu Karang'!G14</f>
-        <v>2</v>
-      </c>
-      <c r="C14" s="27">
-        <f>'Padang Lamun'!G14</f>
-        <v>1</v>
-      </c>
-      <c r="D14" s="27">
-        <f>'Luas Mangove'!F14</f>
-        <v>1</v>
-      </c>
-      <c r="E14" s="27">
-        <f t="shared" si="1"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="G14" s="27">
-        <f>'Korban Bencana Alam'!H17</f>
-        <v>3</v>
-      </c>
-      <c r="H14" s="27">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J14" s="27">
-        <f>'Indeks Provinsi Membangun'!C14</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="27">
-        <f t="shared" si="0"/>
-        <v>1.4444444444444444</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
+      <c r="I37" s="27">
+        <f>'Korban Bencana Alam'!H21</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="27">
+        <f>IF(COUNT(I37)=0,"",SUM(I37)/COUNT(I37))</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="27">
+        <f>'Indeks Provinsi Membangun'!C18</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="27">
+        <f>(G37+J37+L37)/COUNT(G37,J37,L37)</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A38" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="27">
+        <f>'Luas Terumbu Karang'!G9</f>
+        <v>1</v>
+      </c>
+      <c r="E38" s="27">
+        <f>'Padang Lamun'!G9</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="27">
+        <f>'Luas Mangove'!F9</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="27">
+        <f>IF(COUNT(D38:F38)=0,"",SUM(D38:F38)/COUNT(D38:F38))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I38" s="27">
+        <f>'Korban Bencana Alam'!H12</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="27">
+        <f>IF(COUNT(I38)=0,"",SUM(I38)/COUNT(I38))</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="27">
+        <f>'Indeks Provinsi Membangun'!C9</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="27">
+        <f>(G38+J38+L38)/COUNT(G38,J38,L38)</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="27">
         <f>'Luas Terumbu Karang'!G15</f>
         <v>0</v>
       </c>
-      <c r="C15" s="27" t="str">
+      <c r="E39" s="27" t="str">
         <f>'Padang Lamun'!G15</f>
         <v/>
       </c>
-      <c r="D15" s="27">
+      <c r="F39" s="27">
         <f>'Luas Mangove'!F15</f>
         <v>0</v>
       </c>
-      <c r="E15" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="27">
+      <c r="G39" s="27">
+        <f>IF(COUNT(D39:F39)=0,"",SUM(D39:F39)/COUNT(D39:F39))</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="27">
         <f>'Korban Bencana Alam'!H18</f>
         <v>0</v>
       </c>
-      <c r="H15" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="27">
+      <c r="J39" s="27">
+        <f>IF(COUNT(I39)=0,"",SUM(I39)/COUNT(I39))</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="27">
         <f>'Indeks Provinsi Membangun'!C15</f>
         <v>0</v>
       </c>
-      <c r="N15" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A16" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="27">
-        <f>'Luas Terumbu Karang'!G16</f>
-        <v>2</v>
-      </c>
-      <c r="C16" s="27">
-        <f>'Padang Lamun'!G16</f>
-        <v>1</v>
-      </c>
-      <c r="D16" s="27">
-        <f>'Luas Mangove'!F16</f>
-        <v>2</v>
-      </c>
-      <c r="E16" s="27">
-        <f t="shared" si="1"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="G16" s="27">
-        <f>'Korban Bencana Alam'!H19</f>
-        <v>3</v>
-      </c>
-      <c r="H16" s="27">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J16" s="27">
-        <f>'Indeks Provinsi Membangun'!C16</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="27">
-        <f t="shared" si="0"/>
-        <v>1.5555555555555556</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A17" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="27">
-        <f>'Luas Terumbu Karang'!G17</f>
-        <v>0</v>
-      </c>
-      <c r="C17" s="27">
-        <f>'Padang Lamun'!G17</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="27">
-        <f>'Luas Mangove'!F17</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="27">
-        <f>'Korban Bencana Alam'!H20</f>
-        <v>2</v>
-      </c>
-      <c r="H17" s="27">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J17" s="27">
-        <f>'Indeks Provinsi Membangun'!C17</f>
-        <v>1</v>
-      </c>
-      <c r="N17" s="27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A18" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="27">
-        <f>'Luas Terumbu Karang'!G18</f>
-        <v>1</v>
-      </c>
-      <c r="C18" s="27">
-        <f>'Padang Lamun'!G18</f>
-        <v>1</v>
-      </c>
-      <c r="D18" s="27">
-        <f>'Luas Mangove'!F18</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="27">
-        <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G18" s="27">
-        <f>'Korban Bencana Alam'!H21</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="27">
-        <f>'Indeks Provinsi Membangun'!C18</f>
-        <v>0</v>
-      </c>
-      <c r="N18" s="27">
-        <f t="shared" si="0"/>
-        <v>0.22222222222222221</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A19" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="27">
-        <f>'Luas Terumbu Karang'!G19</f>
-        <v>2</v>
-      </c>
-      <c r="C19" s="27">
-        <f>'Padang Lamun'!G19</f>
-        <v>2</v>
-      </c>
-      <c r="D19" s="27">
-        <f>'Luas Mangove'!F19</f>
-        <v>1</v>
-      </c>
-      <c r="E19" s="27">
-        <f t="shared" si="1"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="G19" s="27">
-        <f>'Korban Bencana Alam'!H22</f>
-        <v>2</v>
-      </c>
-      <c r="H19" s="27">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J19" s="27">
-        <f>'Indeks Provinsi Membangun'!C19</f>
-        <v>0</v>
-      </c>
-      <c r="N19" s="27">
-        <f t="shared" si="0"/>
-        <v>1.2222222222222223</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A20" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="27">
-        <f>'Luas Terumbu Karang'!G20</f>
-        <v>3</v>
-      </c>
-      <c r="C20" s="27">
-        <f>'Padang Lamun'!G20</f>
-        <v>3</v>
-      </c>
-      <c r="D20" s="27">
-        <f>'Luas Mangove'!F20</f>
-        <v>1</v>
-      </c>
-      <c r="E20" s="27">
-        <f t="shared" si="1"/>
-        <v>2.3333333333333335</v>
-      </c>
-      <c r="G20" s="27">
-        <f>'Korban Bencana Alam'!H23</f>
-        <v>2</v>
-      </c>
-      <c r="H20" s="27">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J20" s="27">
-        <f>'Indeks Provinsi Membangun'!C20</f>
-        <v>1</v>
-      </c>
-      <c r="N20" s="27">
-        <f t="shared" si="0"/>
-        <v>1.7777777777777779</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A21" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="27">
-        <f>'Luas Terumbu Karang'!G21</f>
-        <v>3</v>
-      </c>
-      <c r="C21" s="27">
-        <f>'Padang Lamun'!G21</f>
-        <v>3</v>
-      </c>
-      <c r="D21" s="27">
-        <f>'Luas Mangove'!F21</f>
-        <v>3</v>
-      </c>
-      <c r="E21" s="27">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G21" s="27">
-        <f>'Korban Bencana Alam'!H24</f>
-        <v>3</v>
-      </c>
-      <c r="H21" s="27">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J21" s="27">
-        <f>'Indeks Provinsi Membangun'!C21</f>
-        <v>0</v>
-      </c>
-      <c r="N21" s="27">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A22" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="27">
-        <f>'Luas Terumbu Karang'!G22</f>
-        <v>0</v>
-      </c>
-      <c r="C22" s="27">
-        <f>'Padang Lamun'!G22</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="27">
-        <f>'Luas Mangove'!F22</f>
-        <v>2</v>
-      </c>
-      <c r="E22" s="27">
-        <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G22" s="27">
-        <f>'Korban Bencana Alam'!H25</f>
-        <v>3</v>
-      </c>
-      <c r="H22" s="27">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J22" s="27">
-        <f>'Indeks Provinsi Membangun'!C22</f>
-        <v>0</v>
-      </c>
-      <c r="N22" s="27">
-        <f t="shared" si="0"/>
-        <v>1.2222222222222221</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A23" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="27">
-        <f>'Luas Terumbu Karang'!G23</f>
-        <v>1</v>
-      </c>
-      <c r="C23" s="27">
-        <f>'Padang Lamun'!G23</f>
-        <v>1</v>
-      </c>
-      <c r="D23" s="27">
-        <f>'Luas Mangove'!F23</f>
-        <v>2</v>
-      </c>
-      <c r="E23" s="27">
-        <f t="shared" si="1"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="G23" s="27">
-        <f>'Korban Bencana Alam'!H26</f>
-        <v>3</v>
-      </c>
-      <c r="H23" s="27">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J23" s="27">
-        <f>'Indeks Provinsi Membangun'!C23</f>
-        <v>0</v>
-      </c>
-      <c r="N23" s="27">
-        <f t="shared" si="0"/>
-        <v>1.4444444444444444</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A24" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="27">
-        <f>'Luas Terumbu Karang'!G24</f>
-        <v>3</v>
-      </c>
-      <c r="C24" s="27">
-        <f>'Padang Lamun'!G24</f>
-        <v>2</v>
-      </c>
-      <c r="D24" s="27">
-        <f>'Luas Mangove'!F24</f>
-        <v>3</v>
-      </c>
-      <c r="E24" s="27">
-        <f t="shared" si="1"/>
-        <v>2.6666666666666665</v>
-      </c>
-      <c r="G24" s="27">
-        <f>'Korban Bencana Alam'!H27</f>
-        <v>2</v>
-      </c>
-      <c r="H24" s="27">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J24" s="27">
-        <f>'Indeks Provinsi Membangun'!C24</f>
-        <v>0</v>
-      </c>
-      <c r="N24" s="27">
-        <f t="shared" si="0"/>
-        <v>1.5555555555555554</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A25" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="27">
-        <f>'Luas Terumbu Karang'!G25</f>
-        <v>3</v>
-      </c>
-      <c r="C25" s="27">
-        <f>'Padang Lamun'!G25</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="27">
-        <f>'Luas Mangove'!F25</f>
-        <v>3</v>
-      </c>
-      <c r="E25" s="27">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G25" s="27">
-        <f>'Korban Bencana Alam'!H28</f>
-        <v>1</v>
-      </c>
-      <c r="H25" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J25" s="27">
-        <f>'Indeks Provinsi Membangun'!C25</f>
-        <v>1</v>
-      </c>
-      <c r="N25" s="27">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A26" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="27">
-        <f>'Luas Terumbu Karang'!G26</f>
-        <v>1</v>
-      </c>
-      <c r="C26" s="27">
-        <f>'Padang Lamun'!G26</f>
-        <v>3</v>
-      </c>
-      <c r="D26" s="27">
-        <f>'Luas Mangove'!F26</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="27">
-        <f t="shared" si="1"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="G26" s="27">
-        <f>'Korban Bencana Alam'!H29</f>
-        <v>1</v>
-      </c>
-      <c r="H26" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J26" s="27">
-        <f>'Indeks Provinsi Membangun'!C26</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="27">
-        <f t="shared" si="0"/>
-        <v>0.77777777777777768</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="27" t="str">
-        <f>'Luas Terumbu Karang'!G27</f>
-        <v/>
-      </c>
-      <c r="C27" s="27" t="str">
-        <f>'Padang Lamun'!G27</f>
-        <v/>
-      </c>
-      <c r="D27" s="27">
-        <f>'Luas Mangove'!F27</f>
-        <v>1</v>
-      </c>
-      <c r="E27" s="27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G27" s="27">
-        <f>'Korban Bencana Alam'!H30</f>
-        <v>2</v>
-      </c>
-      <c r="H27" s="27">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J27" s="27">
-        <f>'Indeks Provinsi Membangun'!C27</f>
-        <v>0</v>
-      </c>
-      <c r="N27" s="27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A28" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="27">
-        <f>'Luas Terumbu Karang'!G28</f>
-        <v>3</v>
-      </c>
-      <c r="C28" s="27">
-        <f>'Padang Lamun'!G28</f>
-        <v>3</v>
-      </c>
-      <c r="D28" s="27">
-        <f>'Luas Mangove'!F28</f>
-        <v>2</v>
-      </c>
-      <c r="E28" s="27">
-        <f t="shared" si="1"/>
-        <v>2.6666666666666665</v>
-      </c>
-      <c r="G28" s="27">
-        <f>'Korban Bencana Alam'!H31</f>
-        <v>3</v>
-      </c>
-      <c r="H28" s="27">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J28" s="27">
-        <f>'Indeks Provinsi Membangun'!C28</f>
-        <v>0</v>
-      </c>
-      <c r="N28" s="27">
-        <f t="shared" si="0"/>
-        <v>1.8888888888888886</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A29" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="27">
-        <f>'Luas Terumbu Karang'!G29</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="27">
-        <f>'Padang Lamun'!G29</f>
-        <v>2</v>
-      </c>
-      <c r="D29" s="27">
-        <f>'Luas Mangove'!F29</f>
-        <v>2</v>
-      </c>
-      <c r="E29" s="27">
-        <f t="shared" si="1"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="G29" s="27">
-        <f>'Korban Bencana Alam'!H32</f>
-        <v>1</v>
-      </c>
-      <c r="H29" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J29" s="27">
-        <f>'Indeks Provinsi Membangun'!C29</f>
-        <v>1</v>
-      </c>
-      <c r="N29" s="27">
-        <f t="shared" si="0"/>
-        <v>1.1111111111111109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A30" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="27">
-        <f>'Luas Terumbu Karang'!G30</f>
-        <v>2</v>
-      </c>
-      <c r="C30" s="27">
-        <f>'Padang Lamun'!G30</f>
-        <v>2</v>
-      </c>
-      <c r="D30" s="27">
-        <f>'Luas Mangove'!F30</f>
-        <v>1</v>
-      </c>
-      <c r="E30" s="27">
-        <f t="shared" si="1"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="G30" s="27">
-        <f>'Korban Bencana Alam'!H33</f>
-        <v>1</v>
-      </c>
-      <c r="H30" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J30" s="27">
-        <f>'Indeks Provinsi Membangun'!C30</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="27">
-        <f t="shared" si="0"/>
-        <v>0.88888888888888895</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A31" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="27">
-        <f>'Luas Terumbu Karang'!G31</f>
-        <v>1</v>
-      </c>
-      <c r="C31" s="27">
-        <f>'Padang Lamun'!G31</f>
-        <v>1</v>
-      </c>
-      <c r="D31" s="27">
-        <f>'Luas Mangove'!F31</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="27">
-        <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G31" s="27">
-        <f>'Korban Bencana Alam'!H34</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J31" s="27">
-        <f>'Indeks Provinsi Membangun'!C31</f>
-        <v>1</v>
-      </c>
-      <c r="N31" s="27">
-        <f t="shared" si="0"/>
-        <v>0.55555555555555547</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A32" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="27">
-        <f>'Luas Terumbu Karang'!G32</f>
-        <v>3</v>
-      </c>
-      <c r="C32" s="27">
-        <f>'Padang Lamun'!G32</f>
-        <v>3</v>
-      </c>
-      <c r="D32" s="27">
-        <f>'Luas Mangove'!F32</f>
-        <v>3</v>
-      </c>
-      <c r="E32" s="27">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G32" s="27">
-        <f>'Korban Bencana Alam'!H35</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="27">
-        <f>'Indeks Provinsi Membangun'!C32</f>
-        <v>1</v>
-      </c>
-      <c r="N32" s="27">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A33" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="27">
-        <f>'Luas Terumbu Karang'!G33</f>
-        <v>2</v>
-      </c>
-      <c r="C33" s="27">
-        <f>'Padang Lamun'!G33</f>
-        <v>3</v>
-      </c>
-      <c r="D33" s="27">
-        <f>'Luas Mangove'!F33</f>
-        <v>1</v>
-      </c>
-      <c r="E33" s="27">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G33" s="27">
-        <f>'Korban Bencana Alam'!H36</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="27">
-        <f>'Indeks Provinsi Membangun'!C33</f>
-        <v>1</v>
-      </c>
-      <c r="N33" s="27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A34" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="27">
-        <f>'Luas Terumbu Karang'!G34</f>
-        <v>0</v>
-      </c>
-      <c r="C34" s="27">
-        <f>'Padang Lamun'!G34</f>
-        <v>2</v>
-      </c>
-      <c r="D34" s="27">
-        <f>'Luas Mangove'!F34</f>
-        <v>3</v>
-      </c>
-      <c r="E34" s="27">
-        <f t="shared" si="1"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="G34" s="27">
-        <f>'Korban Bencana Alam'!H37</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="27">
-        <f>'Indeks Provinsi Membangun'!C34</f>
-        <v>2</v>
-      </c>
-      <c r="N34" s="27">
-        <f t="shared" si="0"/>
-        <v>1.2222222222222223</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A35" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" s="27" t="str">
-        <f>'Luas Terumbu Karang'!G35</f>
-        <v/>
-      </c>
-      <c r="C35" s="27" t="str">
-        <f>'Padang Lamun'!G35</f>
-        <v/>
-      </c>
-      <c r="D35" s="27">
-        <f>'Luas Mangove'!F35</f>
-        <v>2</v>
-      </c>
-      <c r="E35" s="27">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G35" s="27">
-        <f>'Korban Bencana Alam'!H38</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="27">
-        <f>'Indeks Provinsi Membangun'!C35</f>
-        <v>2</v>
-      </c>
-      <c r="N35" s="27">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A36" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="27">
-        <f>'Luas Terumbu Karang'!G36</f>
-        <v>3</v>
-      </c>
-      <c r="C36" s="27">
-        <f>'Padang Lamun'!G36</f>
-        <v>3</v>
-      </c>
-      <c r="D36" s="27">
-        <f>'Luas Mangove'!F36</f>
-        <v>3</v>
-      </c>
-      <c r="E36" s="27">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G36" s="27">
-        <f>'Korban Bencana Alam'!H39</f>
-        <v>2</v>
-      </c>
-      <c r="H36" s="27">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J36" s="27">
-        <f>'Indeks Provinsi Membangun'!C36</f>
-        <v>2</v>
-      </c>
-      <c r="N36" s="27">
-        <f t="shared" si="0"/>
-        <v>2.3333333333333335</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A37" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="27" t="str">
-        <f>'Luas Terumbu Karang'!G37</f>
-        <v/>
-      </c>
-      <c r="C37" s="27" t="str">
-        <f>'Padang Lamun'!G37</f>
-        <v/>
-      </c>
-      <c r="D37" s="27">
-        <f>'Luas Mangove'!F37</f>
-        <v>3</v>
-      </c>
-      <c r="E37" s="27">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G37" s="27">
-        <f>'Korban Bencana Alam'!H40</f>
-        <v>2</v>
-      </c>
-      <c r="H37" s="27">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J37" s="27">
-        <f>'Indeks Provinsi Membangun'!C37</f>
-        <v>2</v>
-      </c>
-      <c r="N37" s="27">
-        <f t="shared" si="0"/>
-        <v>2.3333333333333335</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="27" t="str">
-        <f>'Luas Terumbu Karang'!G38</f>
-        <v/>
-      </c>
-      <c r="C38" s="27" t="str">
-        <f>'Padang Lamun'!G38</f>
-        <v/>
-      </c>
-      <c r="D38" s="27">
-        <f>'Luas Mangove'!F38</f>
-        <v>3</v>
-      </c>
-      <c r="E38" s="27">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G38" s="27">
-        <f>'Korban Bencana Alam'!H41</f>
-        <v>1</v>
-      </c>
-      <c r="H38" s="27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J38" s="27">
-        <f>'Indeks Provinsi Membangun'!C38</f>
-        <v>3</v>
-      </c>
-      <c r="N38" s="27">
-        <f t="shared" si="0"/>
-        <v>2.3333333333333335</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A39" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="27" t="str">
-        <f>'Luas Terumbu Karang'!G39</f>
-        <v/>
-      </c>
-      <c r="C39" s="27" t="str">
-        <f>'Padang Lamun'!G39</f>
-        <v/>
-      </c>
-      <c r="D39" s="27" t="str">
-        <f>'Luas Mangove'!F39</f>
-        <v/>
-      </c>
-      <c r="E39" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G39" s="27">
-        <f>'Korban Bencana Alam'!H42</f>
-        <v>2</v>
-      </c>
-      <c r="H39" s="27">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J39" s="27">
-        <f>'Indeks Provinsi Membangun'!C39</f>
-        <v>3</v>
-      </c>
-      <c r="N39" s="27">
-        <f>SUM(E39,H39,J39)/COUNT(E39,H39,J39)</f>
-        <v>2.5</v>
+      <c r="P39" s="27">
+        <f>(G39+J39+L39)/COUNT(G39,J39,L39)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A39">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:P39">
+    <sortCondition descending="1" ref="P1:P39"/>
+  </sortState>
+  <conditionalFormatting sqref="A2:C39">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>"COUNT($B$2:$J$2)=7"</formula>
     </cfRule>
@@ -17361,16 +17453,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
@@ -17381,6 +17463,16 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
@@ -17397,10 +17489,15 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
@@ -18301,10 +18398,15 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
@@ -19209,11 +19311,13 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" customWidth="1"/>
   </cols>

</xml_diff>